<commit_message>
KW BB League Helper -  Cleaned template
</commit_message>
<xml_diff>
--- a/samples/clean/Hoja limpia Acta.xlsx
+++ b/samples/clean/Hoja limpia Acta.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/cgimeno/Documents/Workspace/KW BB League/samples/clean/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FEB650F4-5EBB-8542-95BF-9CA27DAE238D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92DAA954-11E7-164E-8EB5-B55C7603E7A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="76800" yWindow="620" windowWidth="76800" windowHeight="42580" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="1180" windowWidth="54080" windowHeight="33940" tabRatio="500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
   <si>
     <t>NOMBRE EQUIPO 1</t>
   </si>
@@ -280,7 +280,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="22">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -339,9 +339,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -678,10 +675,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C1005"/>
+  <dimension ref="A1:C999"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="A31" sqref="A31:XFD36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="32.83203125" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
@@ -842,45 +839,24 @@
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
     </row>
-    <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B31" s="1"/>
-      <c r="C31" s="1"/>
-    </row>
-    <row r="32" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B32" s="4"/>
-      <c r="C32" s="4"/>
-    </row>
-    <row r="33" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A33" s="10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B33" s="1"/>
-      <c r="C33" s="1"/>
-    </row>
-    <row r="34" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="B34" s="4"/>
-      <c r="C34" s="4"/>
-    </row>
-    <row r="35" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15">
-      <c r="A35" s="10" t="s">
-        <v>10</v>
-      </c>
-      <c r="B35" s="21"/>
-      <c r="C35" s="21"/>
-    </row>
-    <row r="36" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="37" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="38" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="39" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="40" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="41" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="42" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="43" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="44" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="45" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="46" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="47" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="48" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="31" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="32" spans="1:3" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="33" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="34" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="35" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="36" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="37" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="38" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="39" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="40" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="41" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="42" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="43" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="44" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="45" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="46" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="47" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
+    <row r="48" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="49" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="50" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="51" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
@@ -1832,16 +1808,7 @@
     <row r="997" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="998" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
     <row r="999" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1000" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1001" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1002" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1003" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1004" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
-    <row r="1005" ht="12.75" customHeight="1" x14ac:dyDescent="0.15"/>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B35:C35"/>
-  </mergeCells>
   <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0" footer="0"/>
   <pageSetup paperSize="9" orientation="landscape" horizontalDpi="300" verticalDpi="300"/>
   <headerFooter>

</xml_diff>